<commit_message>
Add function write_out_data. It write result data in xlxs.
</commit_message>
<xml_diff>
--- a/count.xlsx
+++ b/count.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,7 +392,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>